<commit_message>
add bwaise uncertainty models and docs
</commit_message>
<xml_diff>
--- a/qsdsan/systems/bwaise/results/sysA.xlsx
+++ b/qsdsan/systems/bwaise/results/sysA.xlsx
@@ -120,123 +120,123 @@
     <t>Cumulative NPV [MM$]</t>
   </si>
   <si>
+    <t>A8_N2O</t>
+  </si>
+  <si>
+    <t>A2_N2O</t>
+  </si>
+  <si>
+    <t>liq</t>
+  </si>
+  <si>
+    <t>feces</t>
+  </si>
+  <si>
+    <t>desiccant</t>
+  </si>
+  <si>
+    <t>anaerobic_treated</t>
+  </si>
+  <si>
+    <t>A7_N2O</t>
+  </si>
+  <si>
+    <t>A_sol_N</t>
+  </si>
+  <si>
+    <t>A_sol_non_fertilizers</t>
+  </si>
+  <si>
+    <t>A6_CH4</t>
+  </si>
+  <si>
+    <t>A_CH4</t>
+  </si>
+  <si>
+    <t>mixed_waste</t>
+  </si>
+  <si>
+    <t>sol</t>
+  </si>
+  <si>
+    <t>dried_sludge</t>
+  </si>
+  <si>
+    <t>A_liq_non_fertilizers</t>
+  </si>
+  <si>
+    <t>A_liq_P</t>
+  </si>
+  <si>
+    <t>toilet_paper</t>
+  </si>
+  <si>
+    <t>liquid_fertilizer</t>
+  </si>
+  <si>
+    <t>evaporated</t>
+  </si>
+  <si>
+    <t>leachate</t>
+  </si>
+  <si>
+    <t>A6_N2O</t>
+  </si>
+  <si>
+    <t>transported</t>
+  </si>
+  <si>
+    <t>A_N2O</t>
+  </si>
+  <si>
+    <t>A5_CH4</t>
+  </si>
+  <si>
+    <t>A_sol_P</t>
+  </si>
+  <si>
+    <t>flushing_water</t>
+  </si>
+  <si>
+    <t>A_liq_K</t>
+  </si>
+  <si>
+    <t>urine</t>
+  </si>
+  <si>
+    <t>A2_CH4</t>
+  </si>
+  <si>
+    <t>A8_CH4</t>
+  </si>
+  <si>
     <t>A_liq_N</t>
   </si>
   <si>
-    <t>A2_CH4</t>
+    <t>facultative_treated</t>
+  </si>
+  <si>
+    <t>reuse_loss</t>
+  </si>
+  <si>
+    <t>A5_N2O</t>
+  </si>
+  <si>
+    <t>conveyance_loss</t>
+  </si>
+  <si>
+    <t>cleansing_water</t>
   </si>
   <si>
     <t>ws1</t>
   </si>
   <si>
-    <t>A5_N2O</t>
-  </si>
-  <si>
-    <t>urine</t>
-  </si>
-  <si>
     <t>A7_CH4</t>
   </si>
   <si>
-    <t>A8_CH4</t>
-  </si>
-  <si>
     <t>A_sol_K</t>
   </si>
   <si>
-    <t>cleansing_water</t>
-  </si>
-  <si>
-    <t>feces</t>
-  </si>
-  <si>
-    <t>A_sol_N</t>
-  </si>
-  <si>
-    <t>A7_N2O</t>
-  </si>
-  <si>
-    <t>A_sol_non_fertilizers</t>
-  </si>
-  <si>
-    <t>desiccant</t>
-  </si>
-  <si>
-    <t>liq</t>
-  </si>
-  <si>
-    <t>anaerobic_treated</t>
-  </si>
-  <si>
-    <t>A8_N2O</t>
-  </si>
-  <si>
-    <t>A2_N2O</t>
-  </si>
-  <si>
-    <t>A6_CH4</t>
-  </si>
-  <si>
-    <t>A_CH4</t>
-  </si>
-  <si>
-    <t>A_liq_P</t>
-  </si>
-  <si>
-    <t>A_liq_non_fertilizers</t>
-  </si>
-  <si>
-    <t>dried_sludge</t>
-  </si>
-  <si>
-    <t>mixed_waste</t>
-  </si>
-  <si>
-    <t>sol</t>
-  </si>
-  <si>
-    <t>liquid_fertilizer</t>
-  </si>
-  <si>
-    <t>transported</t>
-  </si>
-  <si>
-    <t>A5_CH4</t>
-  </si>
-  <si>
-    <t>A6_N2O</t>
-  </si>
-  <si>
-    <t>A_N2O</t>
-  </si>
-  <si>
-    <t>A_sol_P</t>
-  </si>
-  <si>
-    <t>toilet_paper</t>
-  </si>
-  <si>
-    <t>leachate</t>
-  </si>
-  <si>
-    <t>evaporated</t>
-  </si>
-  <si>
-    <t>facultative_treated</t>
-  </si>
-  <si>
-    <t>reuse_loss</t>
-  </si>
-  <si>
-    <t>A_liq_K</t>
-  </si>
-  <si>
-    <t>flushing_water</t>
-  </si>
-  <si>
-    <t>conveyance_loss</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -309,34 +309,34 @@
     <t>HAP</t>
   </si>
   <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>liquid</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
     <t>A13</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>liquid</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>gas</t>
+    <t>A9</t>
   </si>
   <si>
     <t>A4</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A12</t>
-  </si>
-  <si>
-    <t>A9</t>
   </si>
   <si>
     <t>Unit Operation</t>
@@ -1203,7 +1203,7 @@
         <v>0.9523809523809523</v>
       </c>
       <c r="Q3">
-        <v>-1.478165454665369</v>
+        <v>-1.47816545466537</v>
       </c>
       <c r="R3">
         <v>-14.29338314216537</v>
@@ -1738,121 +1738,121 @@
         <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
         <v>101</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="O3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" t="s">
         <v>103</v>
       </c>
-      <c r="G3" t="s">
+      <c r="Q3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" t="s">
+        <v>100</v>
+      </c>
+      <c r="S3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="AH3" t="s">
         <v>104</v>
       </c>
-      <c r="J3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3" t="s">
-        <v>104</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="AI3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM3" t="s">
         <v>5</v>
       </c>
-      <c r="N3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O3" t="s">
-        <v>97</v>
-      </c>
-      <c r="P3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>4</v>
-      </c>
-      <c r="R3" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T3" t="s">
-        <v>4</v>
-      </c>
-      <c r="U3" t="s">
-        <v>99</v>
-      </c>
-      <c r="V3" t="s">
-        <v>96</v>
-      </c>
-      <c r="W3" t="s">
-        <v>96</v>
-      </c>
-      <c r="X3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>97</v>
-      </c>
       <c r="AN3" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:40">
@@ -1860,121 +1860,121 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>101</v>
+      </c>
+      <c r="P4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>100</v>
+      </c>
+      <c r="R4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" t="s">
+      <c r="S4" t="s">
+        <v>103</v>
+      </c>
+      <c r="T4" t="s">
+        <v>100</v>
+      </c>
+      <c r="U4" t="s">
+        <v>100</v>
+      </c>
+      <c r="V4" t="s">
+        <v>96</v>
+      </c>
+      <c r="W4" t="s">
+        <v>105</v>
+      </c>
+      <c r="X4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA4" t="s">
         <v>6</v>
       </c>
-      <c r="L4" t="s">
-        <v>97</v>
-      </c>
-      <c r="M4" t="s">
-        <v>102</v>
-      </c>
-      <c r="N4" t="s">
-        <v>97</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="AB4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC4" t="s">
         <v>6</v>
-      </c>
-      <c r="P4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>5</v>
-      </c>
-      <c r="R4" t="s">
-        <v>102</v>
-      </c>
-      <c r="S4" t="s">
-        <v>102</v>
-      </c>
-      <c r="T4" t="s">
-        <v>99</v>
-      </c>
-      <c r="U4" t="s">
-        <v>97</v>
-      </c>
-      <c r="V4" t="s">
-        <v>97</v>
-      </c>
-      <c r="W4" t="s">
-        <v>97</v>
-      </c>
-      <c r="X4" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>99</v>
       </c>
       <c r="AD4" t="s">
         <v>102</v>
       </c>
       <c r="AE4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="AF4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="AG4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK4" t="s">
         <v>6</v>
       </c>
-      <c r="AH4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>97</v>
-      </c>
       <c r="AL4" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="AM4" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="AN4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:40">
@@ -1982,25 +1982,25 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
         <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
         <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
         <v>98</v>
@@ -2009,13 +2009,13 @@
         <v>98</v>
       </c>
       <c r="K5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" t="s">
         <v>98</v>
-      </c>
-      <c r="L5" t="s">
-        <v>98</v>
-      </c>
-      <c r="M5" t="s">
-        <v>100</v>
       </c>
       <c r="N5" t="s">
         <v>98</v>
@@ -2030,28 +2030,28 @@
         <v>98</v>
       </c>
       <c r="R5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="T5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="U5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="V5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="W5" t="s">
         <v>98</v>
       </c>
       <c r="X5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Z5" t="s">
         <v>98</v>
@@ -2063,13 +2063,13 @@
         <v>98</v>
       </c>
       <c r="AC5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AD5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AE5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AF5" t="s">
         <v>98</v>
@@ -2081,7 +2081,7 @@
         <v>98</v>
       </c>
       <c r="AI5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AJ5" t="s">
         <v>98</v>
@@ -2093,7 +2093,7 @@
         <v>98</v>
       </c>
       <c r="AM5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN5" t="s">
         <v>98</v>
@@ -2226,121 +2226,121 @@
         <v>76</v>
       </c>
       <c r="B7">
+        <v>0.01021293548951342</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>11801.0167884562</v>
+      </c>
+      <c r="E7">
+        <v>0.01041666666666667</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>11468.72431455273</v>
+      </c>
+      <c r="H7">
+        <v>0.2976798748463171</v>
+      </c>
+      <c r="I7">
+        <v>1.825957475111844</v>
+      </c>
+      <c r="J7">
+        <v>1117.691921899113</v>
+      </c>
+      <c r="K7">
+        <v>18.65771208211736</v>
+      </c>
+      <c r="L7">
+        <v>70.08777918019197</v>
+      </c>
+      <c r="M7">
+        <v>14075.35273972603</v>
+      </c>
+      <c r="N7">
+        <v>1931.138395890413</v>
+      </c>
+      <c r="O7">
+        <v>1126.874698533487</v>
+      </c>
+      <c r="P7">
+        <v>11278.07439557711</v>
+      </c>
+      <c r="Q7">
+        <v>4.934529836990166</v>
+      </c>
+      <c r="R7">
+        <v>0.000281583</v>
+      </c>
+      <c r="S7">
+        <v>11347.31396883699</v>
+      </c>
+      <c r="T7">
+        <v>652.6847782998941</v>
+      </c>
+      <c r="U7">
+        <v>46151.37064015726</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>13793.84568493152</v>
+      </c>
+      <c r="X7">
+        <v>0.3078928103358305</v>
+      </c>
+      <c r="Y7">
+        <v>4.97353489784605</v>
+      </c>
+      <c r="Z7">
+        <v>3.049287990281032</v>
+      </c>
+      <c r="AA7">
+        <v>0.4166666669999999</v>
+      </c>
+      <c r="AB7">
+        <v>28.25077749748643</v>
+      </c>
+      <c r="AC7">
+        <v>0.05833333333333333</v>
+      </c>
+      <c r="AD7">
+        <v>42.02830025162718</v>
+      </c>
+      <c r="AE7">
+        <v>3.028903542442585</v>
+      </c>
+      <c r="AF7">
         <v>36.05426592540499</v>
       </c>
-      <c r="C7">
-        <v>42.02830025162718</v>
-      </c>
-      <c r="D7">
+      <c r="AG7">
+        <v>11349.64418011353</v>
+      </c>
+      <c r="AH7">
+        <v>2.330211276538965</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>281.5070547945214</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
         <v>13793.84568493152</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0.05833333333333333</v>
-      </c>
-      <c r="G7">
+      <c r="AM7">
         <v>1.399328406158802</v>
       </c>
-      <c r="H7">
-        <v>3.028903542442585</v>
-      </c>
-      <c r="I7">
+      <c r="AN7">
         <v>4.307531168981041</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0.01041666666666667</v>
-      </c>
-      <c r="L7">
-        <v>1.825957475111844</v>
-      </c>
-      <c r="M7">
-        <v>0.2976798748463171</v>
-      </c>
-      <c r="N7">
-        <v>1117.691921899113</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>11801.0167884562</v>
-      </c>
-      <c r="Q7">
-        <v>11468.72431455273</v>
-      </c>
-      <c r="R7">
-        <v>0.01021293548951342</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>18.65771208211736</v>
-      </c>
-      <c r="U7">
-        <v>70.08777918019197</v>
-      </c>
-      <c r="V7">
-        <v>4.934529836990166</v>
-      </c>
-      <c r="W7">
-        <v>11278.07439557711</v>
-      </c>
-      <c r="X7">
-        <v>1126.874698533487</v>
-      </c>
-      <c r="Y7">
-        <v>14075.35273972603</v>
-      </c>
-      <c r="Z7">
-        <v>1931.138395890413</v>
-      </c>
-      <c r="AA7">
-        <v>11347.31396883699</v>
-      </c>
-      <c r="AB7">
-        <v>13793.84568493152</v>
-      </c>
-      <c r="AC7">
-        <v>4.97353489784605</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>0.3078928103358305</v>
-      </c>
-      <c r="AF7">
-        <v>3.049287990281032</v>
-      </c>
-      <c r="AG7">
-        <v>0.000281583</v>
-      </c>
-      <c r="AH7">
-        <v>46151.37064015726</v>
-      </c>
-      <c r="AI7">
-        <v>652.6847782998941</v>
-      </c>
-      <c r="AJ7">
-        <v>11349.64418011353</v>
-      </c>
-      <c r="AK7">
-        <v>2.330211276538965</v>
-      </c>
-      <c r="AL7">
-        <v>28.25077749748643</v>
-      </c>
-      <c r="AM7">
-        <v>0.4166666669999999</v>
-      </c>
-      <c r="AN7">
-        <v>281.5070547945214</v>
       </c>
     </row>
     <row r="8" spans="1:40">
@@ -2353,121 +2353,121 @@
         <v>78</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.1947287859832708</v>
+      </c>
+      <c r="E9">
+        <v>0.06574463999999999</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0.2003708180227447</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0.1665958663793535</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0.09326801448885307</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0.03670593194421815</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0.1665958663793535</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0.3659002285714285</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
         <v>29.3541254131959</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
+      <c r="AG9">
+        <v>0.09815670052917135</v>
+      </c>
+      <c r="AH9">
+        <v>23.90434799016876</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0.1665958663793533</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
         <v>0.1665958663793535</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0.3659002285714285</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0.06574463999999999</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0.1947287859832708</v>
-      </c>
-      <c r="Q9">
-        <v>0.2003708180227447</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0.1665958663793535</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0.09326801448885307</v>
-      </c>
-      <c r="AB9">
-        <v>0.1665958663793535</v>
-      </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9">
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-      <c r="AG9">
-        <v>0</v>
-      </c>
-      <c r="AH9">
-        <v>0.03670593194421815</v>
-      </c>
-      <c r="AI9">
-        <v>0</v>
-      </c>
-      <c r="AJ9">
-        <v>0.09815670052917135</v>
-      </c>
-      <c r="AK9">
-        <v>23.90434799016876</v>
-      </c>
-      <c r="AL9">
-        <v>0</v>
-      </c>
       <c r="AM9">
         <v>0</v>
       </c>
       <c r="AN9">
-        <v>0.1665958663793533</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:40">
@@ -2475,121 +2475,121 @@
         <v>79</v>
       </c>
       <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.220240893225146</v>
+      </c>
+      <c r="E10">
+        <v>0.26297856</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0.2266221078447728</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0.2110829066666666</v>
+      </c>
+      <c r="N10">
+        <v>0.1618623313054371</v>
+      </c>
+      <c r="O10">
+        <v>0.162037312354971</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0.2244659093667874</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0.2110829066666666</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0.06457062857142859</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
         <v>70.6458745868041</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
+      <c r="AG10">
+        <v>0.2289998203651648</v>
+      </c>
+      <c r="AH10">
+        <v>22.30756073170247</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0.2110829066666669</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
         <v>0.2110829066666666</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0.06457062857142859</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0.26297856</v>
-      </c>
-      <c r="L10">
-        <v>100</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0.220240893225146</v>
-      </c>
-      <c r="Q10">
-        <v>0.2266221078447728</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>0.162037312354971</v>
-      </c>
-      <c r="Y10">
-        <v>0.2110829066666666</v>
-      </c>
-      <c r="Z10">
-        <v>0.1618623313054371</v>
-      </c>
-      <c r="AA10">
-        <v>0.2244659093667874</v>
-      </c>
-      <c r="AB10">
-        <v>0.2110829066666666</v>
-      </c>
-      <c r="AC10">
-        <v>0</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
-      </c>
-      <c r="AI10">
-        <v>0</v>
-      </c>
-      <c r="AJ10">
-        <v>0.2289998203651648</v>
-      </c>
-      <c r="AK10">
-        <v>22.30756073170247</v>
-      </c>
-      <c r="AL10">
-        <v>0</v>
-      </c>
       <c r="AM10">
         <v>0</v>
       </c>
       <c r="AN10">
-        <v>0.2110829066666669</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:40">
@@ -2603,115 +2603,115 @@
         <v>0</v>
       </c>
       <c r="D11">
+        <v>0.1066695060646485</v>
+      </c>
+      <c r="E11">
+        <v>0.15953652</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0.1097601265284525</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0.1133648633333333</v>
+      </c>
+      <c r="N11">
+        <v>0.157901059642857</v>
+      </c>
+      <c r="O11">
+        <v>0.2705968990384974</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0.0434863250505081</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0.007589476234595889</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
         <v>0.1133648633333332</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>100</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
         <v>0.04455919285714285</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0.15953652</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0.1066695060646485</v>
-      </c>
-      <c r="Q11">
-        <v>0.1097601265284525</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>100</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0.2705968990384974</v>
-      </c>
-      <c r="Y11">
-        <v>0.1133648633333333</v>
-      </c>
-      <c r="Z11">
-        <v>0.157901059642857</v>
-      </c>
-      <c r="AA11">
-        <v>0.0434863250505081</v>
-      </c>
-      <c r="AB11">
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0.04436469062495859</v>
+      </c>
+      <c r="AH11">
+        <v>4.321697846231136</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0.1133648633333339</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
         <v>0.1133648633333332</v>
       </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>100</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0.007589476234595889</v>
-      </c>
-      <c r="AI11">
-        <v>0</v>
-      </c>
-      <c r="AJ11">
-        <v>0.04436469062495859</v>
-      </c>
-      <c r="AK11">
-        <v>4.321697846231136</v>
-      </c>
-      <c r="AL11">
-        <v>0</v>
-      </c>
       <c r="AM11">
         <v>0</v>
       </c>
       <c r="AN11">
-        <v>0.1133648633333339</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:40">
@@ -2725,115 +2725,115 @@
         <v>0</v>
       </c>
       <c r="D12">
+        <v>0.2442783066390175</v>
+      </c>
+      <c r="E12">
+        <v>0.23392512</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0.2513559763612752</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0.2402147733333333</v>
+      </c>
+      <c r="N12">
+        <v>0.2230565752380951</v>
+      </c>
+      <c r="O12">
+        <v>0.3822546707798883</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0.2489644472257596</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0.01947451275169619</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
         <v>0.2402147733333332</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>100</v>
+      </c>
+      <c r="AC12">
         <v>0.1188905142857143</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0.253993195905976</v>
+      </c>
+      <c r="AH12">
+        <v>24.7422405575548</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0.2402147733333323</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>0.2402147733333332</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
         <v>100</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0.23392512</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0.2442783066390175</v>
-      </c>
-      <c r="Q12">
-        <v>0.2513559763612752</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0.3822546707798883</v>
-      </c>
-      <c r="Y12">
-        <v>0.2402147733333333</v>
-      </c>
-      <c r="Z12">
-        <v>0.2230565752380951</v>
-      </c>
-      <c r="AA12">
-        <v>0.2489644472257596</v>
-      </c>
-      <c r="AB12">
-        <v>0.2402147733333332</v>
-      </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12">
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <v>0.01947451275169619</v>
-      </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <v>0.253993195905976</v>
-      </c>
-      <c r="AK12">
-        <v>24.7422405575548</v>
-      </c>
-      <c r="AL12">
-        <v>100</v>
-      </c>
-      <c r="AM12">
-        <v>0</v>
-      </c>
-      <c r="AN12">
-        <v>0.2402147733333323</v>
       </c>
     </row>
     <row r="13" spans="1:40">
@@ -2847,115 +2847,115 @@
         <v>0</v>
       </c>
       <c r="D13">
+        <v>0.05119647330652067</v>
+      </c>
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.05267982945874502</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0.2102146100338443</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0.06083333333333331</v>
+      </c>
+      <c r="N13">
+        <v>0.1216666666666666</v>
+      </c>
+      <c r="O13">
+        <v>0.2085015945479744</v>
+      </c>
+      <c r="P13">
+        <v>0.05249894719724466</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0.05217860665581671</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
         <v>0.0608333333333333</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
         <v>0.01428571428571429</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0.1</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0.2102146100338443</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0.05119647330652067</v>
-      </c>
-      <c r="Q13">
-        <v>0.05267982945874502</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>0.05249894719724466</v>
-      </c>
-      <c r="X13">
-        <v>0.2085015945479744</v>
-      </c>
-      <c r="Y13">
-        <v>0.06083333333333331</v>
-      </c>
-      <c r="Z13">
-        <v>0.1216666666666666</v>
-      </c>
-      <c r="AA13">
-        <v>0.05217860665581671</v>
-      </c>
-      <c r="AB13">
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0.05323254468704906</v>
+      </c>
+      <c r="AH13">
+        <v>5.185542161630679</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0.06083333333333325</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
         <v>0.0608333333333333</v>
       </c>
-      <c r="AC13">
-        <v>0</v>
-      </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
-      <c r="AG13">
-        <v>0</v>
-      </c>
-      <c r="AH13">
-        <v>0</v>
-      </c>
-      <c r="AI13">
-        <v>0</v>
-      </c>
-      <c r="AJ13">
-        <v>0.05323254468704906</v>
-      </c>
-      <c r="AK13">
-        <v>5.185542161630679</v>
-      </c>
-      <c r="AL13">
-        <v>0</v>
-      </c>
       <c r="AM13">
         <v>0</v>
       </c>
       <c r="AN13">
-        <v>0.06083333333333325</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:40">
@@ -2969,115 +2969,115 @@
         <v>0</v>
       </c>
       <c r="D14">
+        <v>0.1929032549771618</v>
+      </c>
+      <c r="E14">
+        <v>0.7599999999999999</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.1984923944544318</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>1.600300428130661</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>0.2947037037037035</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
+      <c r="N14">
+        <v>0.9262116402116389</v>
+      </c>
+      <c r="O14">
+        <v>1.587259757860452</v>
+      </c>
+      <c r="P14">
+        <v>0.1978108479580132</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0.1966038364364847</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0.2947037037037035</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
         <v>0.02</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0.7599999999999999</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>1.600300428130661</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0.1929032549771618</v>
-      </c>
-      <c r="Q14">
-        <v>0.1984923944544318</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0.1978108479580132</v>
-      </c>
-      <c r="X14">
-        <v>1.587259757860452</v>
-      </c>
-      <c r="Y14">
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0.2005749708455231</v>
+      </c>
+      <c r="AH14">
+        <v>19.53861071271215</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0.2947037037037036</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
         <v>0.2947037037037035</v>
       </c>
-      <c r="Z14">
-        <v>0.9262116402116389</v>
-      </c>
-      <c r="AA14">
-        <v>0.1966038364364847</v>
-      </c>
-      <c r="AB14">
-        <v>0.2947037037037035</v>
-      </c>
-      <c r="AC14">
-        <v>0</v>
-      </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
-      <c r="AE14">
-        <v>0</v>
-      </c>
-      <c r="AF14">
-        <v>0</v>
-      </c>
-      <c r="AG14">
-        <v>0</v>
-      </c>
-      <c r="AH14">
-        <v>0</v>
-      </c>
-      <c r="AI14">
-        <v>0</v>
-      </c>
-      <c r="AJ14">
-        <v>0.2005749708455231</v>
-      </c>
-      <c r="AK14">
-        <v>19.53861071271215</v>
-      </c>
-      <c r="AL14">
-        <v>0</v>
-      </c>
       <c r="AM14">
         <v>0</v>
       </c>
       <c r="AN14">
-        <v>0.2947037037037036</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:40">
@@ -3091,115 +3091,115 @@
         <v>0</v>
       </c>
       <c r="D15">
+        <v>93.89956205165797</v>
+      </c>
+      <c r="E15">
+        <v>85</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>96.6201887680056</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>74.68265472433458</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
         <v>91.11679328808579</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="N15">
+        <v>77.02227765647899</v>
+      </c>
+      <c r="O15">
+        <v>74.07407407407406</v>
+      </c>
+      <c r="P15">
+        <v>98.25350226762684</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>97.65397443337616</v>
+      </c>
+      <c r="T15">
+        <v>100</v>
+      </c>
+      <c r="U15">
+        <v>99.93623007906949</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>91.11679328808579</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>100</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
         <v>94.99999999999999</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>85</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>74.68265472433458</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>93.89956205165797</v>
-      </c>
-      <c r="Q15">
-        <v>96.6201887680056</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <v>98.25350226762684</v>
-      </c>
-      <c r="X15">
-        <v>74.07407407407406</v>
-      </c>
-      <c r="Y15">
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>97.63392495968235</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
         <v>91.11679328808579</v>
       </c>
-      <c r="Z15">
-        <v>77.02227765647899</v>
-      </c>
-      <c r="AA15">
-        <v>97.65397443337616</v>
-      </c>
-      <c r="AB15">
+      <c r="AK15">
+        <v>0</v>
+      </c>
+      <c r="AL15">
         <v>91.11679328808579</v>
       </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15">
-        <v>0</v>
-      </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
-      <c r="AG15">
-        <v>0</v>
-      </c>
-      <c r="AH15">
-        <v>99.93623007906949</v>
-      </c>
-      <c r="AI15">
-        <v>100</v>
-      </c>
-      <c r="AJ15">
-        <v>97.63392495968235</v>
-      </c>
-      <c r="AK15">
-        <v>0</v>
-      </c>
-      <c r="AL15">
-        <v>0</v>
-      </c>
       <c r="AM15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AN15">
-        <v>91.11679328808579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:40">
@@ -3213,115 +3213,115 @@
         <v>0</v>
       </c>
       <c r="D16">
+        <v>4.022564687918848</v>
+      </c>
+      <c r="E16">
+        <v>13.41781515999999</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1.241734096473468</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>23.50683023750091</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>6.8828308651645</v>
+      </c>
+      <c r="N16">
+        <v>21.38702407045631</v>
+      </c>
+      <c r="O16">
+        <v>23.31527569134414</v>
+      </c>
+      <c r="P16">
+        <v>0.3788174875850964</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0.3765060012495807</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
         <v>6.882830865164499</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
         <v>4.371793721428576</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>13.41781515999999</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>23.50683023750091</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>4.022564687918848</v>
-      </c>
-      <c r="Q16">
-        <v>1.241734096473468</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <v>0.3788174875850964</v>
-      </c>
-      <c r="X16">
-        <v>23.31527569134414</v>
-      </c>
-      <c r="Y16">
-        <v>6.8828308651645</v>
-      </c>
-      <c r="Z16">
-        <v>21.38702407045631</v>
-      </c>
-      <c r="AA16">
-        <v>0.3765060012495807</v>
-      </c>
-      <c r="AB16">
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0.3764287002773323</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <v>6.882830865164502</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
         <v>6.882830865164499</v>
       </c>
-      <c r="AC16">
-        <v>0</v>
-      </c>
-      <c r="AD16">
-        <v>0</v>
-      </c>
-      <c r="AE16">
-        <v>0</v>
-      </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
-      <c r="AG16">
-        <v>0</v>
-      </c>
-      <c r="AH16">
-        <v>0</v>
-      </c>
-      <c r="AI16">
-        <v>0</v>
-      </c>
-      <c r="AJ16">
-        <v>0.3764287002773323</v>
-      </c>
-      <c r="AK16">
-        <v>0</v>
-      </c>
-      <c r="AL16">
-        <v>0</v>
-      </c>
       <c r="AM16">
         <v>0</v>
       </c>
       <c r="AN16">
-        <v>6.882830865164502</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:40">
@@ -3329,7 +3329,7 @@
         <v>86</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -3362,41 +3362,41 @@
         <v>0</v>
       </c>
       <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
         <v>100</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>100</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
       <c r="Y17">
         <v>0</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="AE17">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AF17">
         <v>0</v>
@@ -3454,115 +3454,115 @@
         <v>0</v>
       </c>
       <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>100</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
+      <c r="L18">
+        <v>99.99999999999999</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
         <v>100</v>
       </c>
-      <c r="H18">
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
         <v>100</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
+      <c r="AE18">
         <v>100</v>
       </c>
-      <c r="U18">
-        <v>99.99999999999999</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18">
-        <v>0</v>
-      </c>
-      <c r="AB18">
-        <v>0</v>
-      </c>
-      <c r="AC18">
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
         <v>100</v>
-      </c>
-      <c r="AD18">
-        <v>0</v>
-      </c>
-      <c r="AE18">
-        <v>0</v>
-      </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
-      <c r="AG18">
-        <v>0</v>
-      </c>
-      <c r="AH18">
-        <v>0</v>
-      </c>
-      <c r="AI18">
-        <v>0</v>
-      </c>
-      <c r="AJ18">
-        <v>0</v>
-      </c>
-      <c r="AK18">
-        <v>0</v>
-      </c>
-      <c r="AL18">
-        <v>0</v>
-      </c>
-      <c r="AM18">
-        <v>0</v>
       </c>
       <c r="AN18">
         <v>0</v>
@@ -4067,115 +4067,115 @@
         <v>0</v>
       </c>
       <c r="D23">
+        <v>1.067856040227408</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1.098795882850504</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0.9135803999999997</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>1.117370449632785</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>100</v>
+      </c>
+      <c r="S23">
+        <v>1.110552426150026</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
         <v>0.9135803999999996</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>1.067856040227408</v>
-      </c>
-      <c r="Q23">
-        <v>1.098795882850504</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="W23">
-        <v>1.117370449632785</v>
-      </c>
       <c r="X23">
         <v>0</v>
       </c>
       <c r="Y23">
-        <v>0.9135803999999997</v>
+        <v>0</v>
       </c>
       <c r="Z23">
         <v>0</v>
       </c>
       <c r="AA23">
-        <v>1.110552426150026</v>
+        <v>0</v>
       </c>
       <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>1.11032441708247</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0.9135803999999959</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
         <v>0.9135803999999996</v>
       </c>
-      <c r="AC23">
-        <v>0</v>
-      </c>
-      <c r="AD23">
-        <v>0</v>
-      </c>
-      <c r="AE23">
-        <v>0</v>
-      </c>
-      <c r="AF23">
-        <v>0</v>
-      </c>
-      <c r="AG23">
-        <v>100</v>
-      </c>
-      <c r="AH23">
-        <v>0</v>
-      </c>
-      <c r="AI23">
-        <v>0</v>
-      </c>
-      <c r="AJ23">
-        <v>1.11032441708247</v>
-      </c>
-      <c r="AK23">
-        <v>0</v>
-      </c>
-      <c r="AL23">
-        <v>0</v>
-      </c>
       <c r="AM23">
         <v>0</v>
       </c>
       <c r="AN23">
-        <v>0.9135803999999959</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:40">

</xml_diff>